<commit_message>
Entry 2 for Angus
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-9417-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-9417-350-1201.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t xml:space="preserve">Started reading about the file structure and implementation of the Logic Unit and set up Quartus </t>
+  </si>
+  <si>
+    <t>30/03/2020</t>
+  </si>
+  <si>
+    <t>8:30pm</t>
+  </si>
+  <si>
+    <t>Finished Logic Unit Design</t>
   </si>
 </sst>
 </file>
@@ -663,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,18 +746,28 @@
         <v>8</v>
       </c>
       <c r="E6" s="21">
-        <v>0.4513888888888889</v>
+        <v>0.95138888888888884</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="22"/>
-      <c r="G7" s="13"/>
+      <c r="B7" s="13">
+        <v>9417</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>

</xml_diff>

<commit_message>
Worked on arithmatic unit
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-9417-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-9417-350-1201.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>Finished Logic Unit Design</t>
+  </si>
+  <si>
+    <t>31/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:45pm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:25PM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on the Arithmatic unit </t>
   </si>
 </sst>
 </file>
@@ -673,7 +685,7 @@
   <dimension ref="A1:G756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,11 +782,21 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="22"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="13">
+        <v>9417</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>

</xml_diff>

<commit_message>
Synthesized both units as well as completed the timing simulations
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-9417-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-9417-350-1201.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Finished the arithmatic unit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synthesized both the Arithmetic unit and Logic unit, as well as completed the timing simulations for both </t>
   </si>
 </sst>
 </file>
@@ -678,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +800,7 @@
         <v>9417</v>
       </c>
       <c r="C9" s="10">
-        <v>43834</v>
+        <v>43922</v>
       </c>
       <c r="D9" s="19">
         <v>0.86111111111111116</v>
@@ -810,11 +813,21 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22"/>
-      <c r="G10" s="13"/>
+      <c r="B10" s="13">
+        <v>9417</v>
+      </c>
+      <c r="C10" s="10">
+        <v>43923</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>

</xml_diff>